<commit_message>
After changes on 4-2-2024; 1. I added an “Exceptions” tab that reports on all the POs marked as “materials” during the time frame of the report a. This included having to import these from Yardi so we can report on them, where before we were not even importing these from Yardi 2. I renamed the report to show the date range of the report in the file name 3. Removed “Cabinets” Category from the report 4. Not seen in this report, but I made the code changes so we can accept the ADP reports with the headers in the first row instead of the 5th row
</commit_message>
<xml_diff>
--- a/LW_Web/_Templates/_Template - Inventory Daily Pivot_WithDollars.xlsx
+++ b/LW_Web/_Templates/_Template - Inventory Daily Pivot_WithDollars.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent\Source\Repos\lemlewolff\LW_Web\_Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CAA273C-42D9-4D78-999C-39D6A25D91CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BB4594-91BC-4B10-94ED-A9BD6386E55C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2265" yWindow="765" windowWidth="26325" windowHeight="14625" tabRatio="429" activeTab="1" xr2:uid="{EA24823F-ADC4-41EB-9C5B-69E077F92E78}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="429" activeTab="1" xr2:uid="{EA24823F-ADC4-41EB-9C5B-69E077F92E78}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Full Inventory" sheetId="7" r:id="rId3"/>
     <sheet name="Labor" sheetId="4" r:id="rId4"/>
     <sheet name="LaborPO" sheetId="6" r:id="rId5"/>
+    <sheet name="Exceptions" sheetId="8" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Detail!$A$1:$H$252</definedName>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>Report Start Date</t>
   </si>
@@ -112,6 +113,36 @@
   </si>
   <si>
     <t>Category</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>QtyOrdered</t>
+  </si>
+  <si>
+    <t>UnitPrice</t>
+  </si>
+  <si>
+    <t>TotalCost</t>
+  </si>
+  <si>
+    <t>OrderDate</t>
+  </si>
+  <si>
+    <t>ReceivedDate</t>
+  </si>
+  <si>
+    <t>ItemCode</t>
+  </si>
+  <si>
+    <t>ItemDesc</t>
+  </si>
+  <si>
+    <t>ExpenseType</t>
+  </si>
+  <si>
+    <t>Client</t>
   </si>
 </sst>
 </file>
@@ -125,7 +156,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +203,15 @@
       <family val="2"/>
       <charset val="161"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="161"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -289,7 +329,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -353,6 +393,8 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -383,6 +425,81 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1965960</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>373380</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C6AF76B-650A-1962-771C-CD13F8217EEC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="76200" y="53340"/>
+          <a:ext cx="3352800" cy="320040"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Exceptions is when Item Code = "Materials"</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -685,18 +802,18 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" style="9" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="9" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -708,13 +825,13 @@
       </c>
       <c r="D1" s="12"/>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="15"/>
       <c r="D2" s="13"/>
     </row>
-    <row r="4" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -741,19 +858,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" customWidth="1"/>
-    <col min="3" max="3" width="34.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" style="9" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="8" customWidth="1"/>
-    <col min="8" max="14" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" customWidth="1"/>
+    <col min="3" max="3" width="34.44140625" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" style="9" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" style="8" customWidth="1"/>
+    <col min="8" max="14" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="26" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="26" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>7</v>
       </c>
@@ -782,7 +899,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="7" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="7" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H2" s="7" t="e">
         <f>IF(ISERR(INT(RIGHT(H1,6))),  _xlfn.XLOOKUP(INT(RIGHT(H1,5)),LaborPO!$A:$A,LaborPO!$B:$B,"PO Not Listed",0,2), _xlfn.XLOOKUP(INT(RIGHT(H1,6)),Labor!$A:$A,Labor!$B:$B,"Not Listed",0,2))</f>
         <v>#VALUE!</v>
@@ -807,19 +924,19 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="50.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="19" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" style="19" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="50.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" style="19" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" style="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="11" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>8</v>
       </c>
@@ -866,13 +983,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="113.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="113.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="4" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="4" customFormat="1" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
@@ -892,15 +1009,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401A3AB8-DA7F-4E79-B0FB-0C8635ECB629}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" style="6" customWidth="1"/>
     <col min="2" max="2" width="146" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="4" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="4" customFormat="1" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -911,4 +1030,203 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E0A2833-4DD8-4667-9BAC-1A42AB2B023D}">
+  <dimension ref="A1:L34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="11.77734375" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" customWidth="1"/>
+    <col min="10" max="10" width="15.5546875" customWidth="1"/>
+    <col min="11" max="11" width="22.44140625" customWidth="1"/>
+    <col min="12" max="12" width="69.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+    </row>
+    <row r="17" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+    </row>
+    <row r="18" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+    </row>
+    <row r="19" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+    </row>
+    <row r="20" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+    </row>
+    <row r="21" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+    </row>
+    <row r="22" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+    </row>
+    <row r="23" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+    </row>
+    <row r="24" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+    </row>
+    <row r="25" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+    </row>
+    <row r="26" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+    </row>
+    <row r="27" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+    </row>
+    <row r="28" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+    </row>
+    <row r="29" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+    </row>
+    <row r="30" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+    </row>
+    <row r="31" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+    </row>
+    <row r="32" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G32" s="27"/>
+      <c r="H32" s="27"/>
+    </row>
+    <row r="33" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
+    </row>
+    <row r="34" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G34" s="27"/>
+      <c r="H34" s="27"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
after removing the Data Processing
</commit_message>
<xml_diff>
--- a/LW_Web/_Templates/_Template - Inventory Daily Pivot_WithDollars.xlsx
+++ b/LW_Web/_Templates/_Template - Inventory Daily Pivot_WithDollars.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent\Source\Repos\lemlewolff\LW_Web\_Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BB4594-91BC-4B10-94ED-A9BD6386E55C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275F1067-A134-4828-9DA6-CA92707F06CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="429" activeTab="1" xr2:uid="{EA24823F-ADC4-41EB-9C5B-69E077F92E78}"/>
   </bookViews>
@@ -22,6 +22,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Detail!$A$1:$H$252</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Full Inventory'!$A$1:$S$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
   <si>
     <t>Report Start Date</t>
   </si>
@@ -97,21 +98,9 @@
     <t>Last Physical Count</t>
   </si>
   <si>
-    <t>Activity Count</t>
-  </si>
-  <si>
-    <t>Total Quantity</t>
-  </si>
-  <si>
-    <t>Total Value</t>
-  </si>
-  <si>
     <t>Last Physical Count Date</t>
   </si>
   <si>
-    <t>* All values are As Of the report End Date</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
@@ -143,20 +132,46 @@
   </si>
   <si>
     <t>Client</t>
+  </si>
+  <si>
+    <t>Total End Quantity</t>
+  </si>
+  <si>
+    <t>item Desc</t>
+  </si>
+  <si>
+    <t>Total Sales</t>
+  </si>
+  <si>
+    <t>Total Purchases</t>
+  </si>
+  <si>
+    <t>Six Mo High</t>
+  </si>
+  <si>
+    <t>Six Mo Low</t>
+  </si>
+  <si>
+    <t>Annualized Turnover</t>
+  </si>
+  <si>
+    <t>Six Mo Avg</t>
+  </si>
+  <si>
+    <t>Total End Value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,14 +201,6 @@
       <name val="Arial Narrow"/>
       <family val="2"/>
       <charset val="161"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="161"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -329,7 +336,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -349,7 +356,6 @@
     <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -366,42 +372,53 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="5" tint="0.39994506668294322"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -814,22 +831,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="12"/>
+      <c r="C1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="11"/>
     </row>
     <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="13"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="4" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -870,32 +887,32 @@
     <col min="8" max="14" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="26" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:9" s="22" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="22" t="s">
         <v>14</v>
       </c>
     </row>
@@ -907,7 +924,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="PO">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="PO">
       <formula>NOT(ISERROR(SEARCH("PO",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -918,55 +935,84 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EA69AD6-A530-4E3F-AC13-64AB42E25366}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.109375" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" customWidth="1"/>
-    <col min="3" max="3" width="50.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" customWidth="1"/>
-    <col min="7" max="7" width="12.44140625" style="19" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" style="19" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="25" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="25" customWidth="1"/>
+    <col min="3" max="3" width="42.44140625" style="25" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.109375" customWidth="1"/>
+    <col min="8" max="8" width="7.21875" customWidth="1"/>
+    <col min="9" max="9" width="8.109375" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" customWidth="1"/>
+    <col min="11" max="11" width="10" customWidth="1"/>
+    <col min="12" max="16" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.33203125" style="27" customWidth="1"/>
+    <col min="19" max="19" width="13.33203125" style="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="11" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:19" s="17" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="20" t="s">
+      <c r="B1" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="18" t="s">
+      <c r="E1" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="R1" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>21</v>
+      <c r="S1" s="26" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G1:H1048576">
+  <conditionalFormatting sqref="A1:B1048576">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"NULL"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"NULL"</formula>
     </cfRule>
@@ -1063,167 +1109,167 @@
         <v>4</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="I1" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
     </row>
     <row r="17" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
     </row>
     <row r="18" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
     </row>
     <row r="19" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
     </row>
     <row r="20" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
     </row>
     <row r="21" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
     </row>
     <row r="22" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
     </row>
     <row r="23" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
     </row>
     <row r="24" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
     </row>
     <row r="25" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
     </row>
     <row r="26" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
     </row>
     <row r="27" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
     </row>
     <row r="28" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
     </row>
     <row r="29" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
     </row>
     <row r="30" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="23"/>
     </row>
     <row r="31" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="23"/>
     </row>
     <row r="32" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G32" s="27"/>
-      <c r="H32" s="27"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
     </row>
     <row r="33" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="23"/>
     </row>
     <row r="34" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G34" s="27"/>
-      <c r="H34" s="27"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Beofre starting USER edit screens
</commit_message>
<xml_diff>
--- a/LW_Web/_Templates/_Template - Inventory Daily Pivot_WithDollars.xlsx
+++ b/LW_Web/_Templates/_Template - Inventory Daily Pivot_WithDollars.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent\Source\Repos\lemlewolff\LW_Web\_Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275F1067-A134-4828-9DA6-CA92707F06CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67F33F8-0850-41CD-8483-1042952995F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="429" activeTab="1" xr2:uid="{EA24823F-ADC4-41EB-9C5B-69E077F92E78}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="458" firstSheet="2" activeTab="6" xr2:uid="{EA24823F-ADC4-41EB-9C5B-69E077F92E78}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -19,9 +19,11 @@
     <sheet name="Labor" sheetId="4" r:id="rId4"/>
     <sheet name="LaborPO" sheetId="6" r:id="rId5"/>
     <sheet name="Exceptions" sheetId="8" r:id="rId6"/>
+    <sheet name="Detail Explained" sheetId="9" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Detail!$A$1:$H$252</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Detail Explained'!$A$1:$G$251</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Full Inventory'!$A$1:$S$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
   <si>
     <t>Report Start Date</t>
   </si>
@@ -159,6 +161,192 @@
   </si>
   <si>
     <t>Total End Value</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="161"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>This is determined from the Item Code.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Take the first two digits of the Item Code (ie, 10-00100 = "10") Then use table tblLookupValues to find the Category Name where the two digit code is in the KeyValue column and the Category name is in the KeyString column where the Cateory column = "invCategoryID" </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="161"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Get the Item Codes from table tblInventoryTracking which is loaded from Sortly and Yardi.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Includes all items with DateOfSale, or ReceivedDate (Yardi Purchase Order "ReceivedDate") from tblInventoryTracking that falls in the report range. As well as any additional items from WorkOrders from Table tblADP (where the PayDate) is in range.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="161"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sortly Item Name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+(tblSortlyInventory.ItemName) or, if that is blank use tblInventoryTracking.ItemDesc (from Yardi Purchase Order mm2podet.sDesc field).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="161"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Last Physical Count of the item</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Quantity (PhysicalCount field) from the table tblPhysicalCounts (Count as of the latest date from before the report start date)</t>
+    </r>
+  </si>
+  <si>
+    <t>sum of tblInventoryTracking Quantity field PLUS the Physical Inventory count (Qty Start)</t>
+  </si>
+  <si>
+    <t>80-02 WO555555 (WO and POs By Date)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="161"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tblSortlyInventory.unitPrice</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> which comes from the Sortly "Price (cost/purchase price)" Field in the export file</t>
+    </r>
+  </si>
+  <si>
+    <t>Sortly Unit Price (Price field (cost/purchase price)) 
+X 
+(tblInventoryTracking Quantities Summed up PLUS the Physical Inventory Count)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Includes all </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="161"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>items</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> with DateOfSale, or ReceivedDate (Yardi Purchase Order "ReceivedDate") from tblInventoryTracking that falls in the report range. As well as any additional items from WorkOrders from Table tblADP (where the PayDate) is in range. 
+The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="161"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>date</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> comes from whichever first is not blank: DateOfSale, ReceivedDate, or ADP PayDate.
+DateOfSale =  the first date from Sortly (WODate) or Yardi (CompleteDate) Yardi Completion Date is the sale date for Supplies/CoOp.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -171,7 +359,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,8 +407,24 @@
       <charset val="161"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="2" tint="-0.499984740745262"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+      <charset val="161"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="161"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -242,6 +446,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -336,7 +546,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -405,13 +615,51 @@
     <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="6" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -511,6 +759,113 @@
             </a:rPr>
             <a:t>Exceptions is when Item Code = "Materials"</a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3124200</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81972150-A930-CEFD-1641-4BB9B930B451}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15041880" y="2796540"/>
+          <a:ext cx="3101340" cy="2270760"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>From John:</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>As for WOs/POs Column- the DateOfSale (?) “Completed Date” from Yardi or Todays WO Date in Sortly only for Repairs/Maintenance or ADP PayDate for both CoOp and Repair/Maintenance (Plumbing in the future) would be used for WO; and the Received Date from Yardi would pertain to all POs. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Note:(Work Completed Date should agree to ADP Pay Date (where applicable) and Sortly’s Todays WO date (where applicable).    </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -871,7 +1226,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDC29F3-B90F-4537-9C7E-93AC43A1A407}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -924,7 +1279,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="PO">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="PO">
       <formula>NOT(ISERROR(SEARCH("PO",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1008,12 +1363,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:B1048576">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"NULL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"NULL"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1275,4 +1630,89 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2534A38F-987B-417D-96DB-24B98916F98B}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="36.6640625" customWidth="1"/>
+    <col min="2" max="2" width="48.44140625" customWidth="1"/>
+    <col min="3" max="3" width="38.21875" customWidth="1"/>
+    <col min="4" max="4" width="24.88671875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="23" style="9" customWidth="1"/>
+    <col min="7" max="7" width="22.44140625" style="8" customWidth="1"/>
+    <col min="8" max="8" width="46.21875" customWidth="1"/>
+    <col min="9" max="13" width="11.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="34" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="35" customFormat="1" ht="184.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:XFD1">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="PO">
+      <formula>NOT(ISERROR(SEARCH("PO",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updates for categories in pivot sheet
</commit_message>
<xml_diff>
--- a/LW_Web/_Templates/_Template - Inventory Daily Pivot_WithDollars.xlsx
+++ b/LW_Web/_Templates/_Template - Inventory Daily Pivot_WithDollars.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent\Source\Repos\lemlewolff\LW_Web\_Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67F33F8-0850-41CD-8483-1042952995F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA2F811-5002-465B-8085-9EE36AC5F284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="458" firstSheet="2" activeTab="6" xr2:uid="{EA24823F-ADC4-41EB-9C5B-69E077F92E78}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="526" activeTab="1" xr2:uid="{EA24823F-ADC4-41EB-9C5B-69E077F92E78}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Detail Explained" sheetId="9" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Detail!$A$1:$H$252</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Detail!$A$1:$H$253</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Detail Explained'!$A$1:$G$251</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Full Inventory'!$A$1:$S$1</definedName>
   </definedNames>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
   <si>
     <t>Report Start Date</t>
   </si>
@@ -348,6 +348,9 @@
 DateOfSale =  the first date from Sortly (WODate) or Yardi (CompleteDate) Yardi Completion Date is the sale date for Supplies/CoOp.</t>
     </r>
   </si>
+  <si>
+    <t>WOCategory</t>
+  </si>
 </sst>
 </file>
 
@@ -359,7 +362,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -423,8 +426,16 @@
       <charset val="161"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+      <charset val="161"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -452,6 +463,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -546,7 +563,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -647,6 +664,21 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="8" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="8" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1224,9 +1256,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDC29F3-B90F-4537-9C7E-93AC43A1A407}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1271,14 +1303,27 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="7" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H2" s="7" t="e">
+    <row r="2" spans="1:9" s="45" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="45" t="str">
+        <f>IF(ISERR(INT(RIGHT(H1,6))), "--", _xlfn.XLOOKUP(INT(RIGHT(H1,6)),Labor!$A:$A,Labor!$C:$C,"Not Listed",0,2))</f>
+        <v>--</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="7" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H3" s="7" t="e">
         <f>IF(ISERR(INT(RIGHT(H1,6))),  _xlfn.XLOOKUP(INT(RIGHT(H1,5)),LaborPO!$A:$A,LaborPO!$B:$B,"PO Not Listed",0,2), _xlfn.XLOOKUP(INT(RIGHT(H1,6)),Labor!$A:$A,Labor!$B:$B,"Not Listed",0,2))</f>
         <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD1">
+  <conditionalFormatting sqref="A1:XFD2">
     <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="PO">
       <formula>NOT(ISERROR(SEARCH("PO",A1)))</formula>
     </cfRule>
@@ -1378,24 +1423,27 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1640E6A9-8949-4063-A1A5-CE5FE939C0A0}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.5546875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="113.33203125" customWidth="1"/>
+    <col min="2" max="2" width="113.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="4" customFormat="1" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>13</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1636,7 +1684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2534A38F-987B-417D-96DB-24B98916F98B}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Starting of Yardi Emailed Imports
</commit_message>
<xml_diff>
--- a/LW_Web/_Templates/_Template - Inventory Daily Pivot_WithDollars.xlsx
+++ b/LW_Web/_Templates/_Template - Inventory Daily Pivot_WithDollars.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent\Source\Repos\lemlewolff\LW_Web\_Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA2F811-5002-465B-8085-9EE36AC5F284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41A6AA5-6597-43B2-81AC-83C1559F48AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="526" activeTab="1" xr2:uid="{EA24823F-ADC4-41EB-9C5B-69E077F92E78}"/>
+    <workbookView xWindow="1008" yWindow="276" windowWidth="17040" windowHeight="12012" tabRatio="526" activeTab="1" xr2:uid="{EA24823F-ADC4-41EB-9C5B-69E077F92E78}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Detail!$A$1:$H$253</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Detail Explained'!$A$1:$G$251</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Full Inventory'!$A$1:$S$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Full Inventory'!$A$1:$T$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -98,9 +98,6 @@
   </si>
   <si>
     <t>Last Physical Count</t>
-  </si>
-  <si>
-    <t>Last Physical Count Date</t>
   </si>
   <si>
     <t>Category</t>
@@ -350,6 +347,9 @@
   </si>
   <si>
     <t>WOCategory</t>
+  </si>
+  <si>
+    <t>Physical Count Date</t>
   </si>
 </sst>
 </file>
@@ -473,7 +473,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -506,45 +506,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -563,7 +524,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -583,20 +544,13 @@
     <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -679,6 +633,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1206,34 +1163,32 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.33203125" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" style="9" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" style="9" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="11"/>
+      <c r="C1"/>
+      <c r="D1"/>
     </row>
     <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="12"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2"/>
+      <c r="D2"/>
     </row>
     <row r="4" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -1274,44 +1229,44 @@
     <col min="8" max="14" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="22" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:9" s="19" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="45" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="41"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="45" t="str">
+    <row r="2" spans="1:9" s="42" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="42" t="str">
         <f>IF(ISERR(INT(RIGHT(H1,6))), "--", _xlfn.XLOOKUP(INT(RIGHT(H1,6)),Labor!$A:$A,Labor!$C:$C,"Not Listed",0,2))</f>
         <v>--</v>
       </c>
@@ -1335,7 +1290,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EA69AD6-A530-4E3F-AC13-64AB42E25366}">
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1343,67 +1298,71 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="25" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" style="25" customWidth="1"/>
-    <col min="3" max="3" width="42.44140625" style="25" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="22" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="22" customWidth="1"/>
+    <col min="3" max="3" width="42.44140625" style="22" customWidth="1"/>
     <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.109375" customWidth="1"/>
-    <col min="8" max="8" width="7.21875" customWidth="1"/>
-    <col min="9" max="9" width="8.109375" customWidth="1"/>
-    <col min="10" max="10" width="11.44140625" customWidth="1"/>
-    <col min="11" max="11" width="10" customWidth="1"/>
-    <col min="12" max="16" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.33203125" style="27" customWidth="1"/>
-    <col min="19" max="19" width="13.33203125" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" style="20" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.109375" customWidth="1"/>
+    <col min="9" max="9" width="7.21875" customWidth="1"/>
+    <col min="10" max="10" width="8.109375" customWidth="1"/>
+    <col min="11" max="11" width="11.44140625" customWidth="1"/>
+    <col min="12" max="12" width="10" customWidth="1"/>
+    <col min="13" max="17" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.33203125" style="24" customWidth="1"/>
+    <col min="20" max="20" width="13.33203125" style="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="17" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:20" s="14" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="28" t="s">
+      <c r="B1" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="17" t="s">
+      <c r="G1" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="H1" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="I1" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="J1" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="S1" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="T1" s="23" t="s">
         <v>36</v>
-      </c>
-      <c r="J1" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="R1" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="S1" s="26" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1443,7 +1402,7 @@
         <v>13</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1512,167 +1471,167 @@
         <v>4</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="J1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
     </row>
     <row r="17" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
     </row>
     <row r="18" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
     </row>
     <row r="19" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
     </row>
     <row r="20" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
     </row>
     <row r="21" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
     </row>
     <row r="22" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
     </row>
     <row r="23" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
     </row>
     <row r="24" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
     </row>
     <row r="25" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G25" s="23"/>
-      <c r="H25" s="23"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
     </row>
     <row r="26" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
     </row>
     <row r="27" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
     </row>
     <row r="28" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
     </row>
     <row r="29" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
     </row>
     <row r="30" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
     </row>
     <row r="31" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
     </row>
     <row r="32" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
     </row>
     <row r="33" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G33" s="23"/>
-      <c r="H33" s="23"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
     </row>
     <row r="34" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G34" s="23"/>
-      <c r="H34" s="23"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1701,56 +1660,56 @@
     <col min="9" max="13" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="34" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:8" s="31" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="32" customFormat="1" ht="184.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="36" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" s="35" customFormat="1" ht="184.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="38" t="s">
+      <c r="E2" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="F2" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" s="37" t="s">
+      <c r="H2" s="32" t="s">
         <v>45</v>
-      </c>
-      <c r="H2" s="35" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>